<commit_message>
few new pdfs added
</commit_message>
<xml_diff>
--- a/Dataset/list.xlsx
+++ b/Dataset/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMFI\1. semester\Bakalárka\na_git\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187A8333-15CB-4C19-8CA3-54BEE1CFEBD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A382FB7F-459E-44C9-81F9-C11EA7996D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="180">
   <si>
     <t>Číslo vložky</t>
   </si>
@@ -451,13 +451,127 @@
   </si>
   <si>
     <t>Mgr. Dagmara Friedmannová, JUDr. Ondrej Matejka</t>
+  </si>
+  <si>
+    <t>test_majitel\7618.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Milan Kučečka, Ing. Marek Gorun</t>
+  </si>
+  <si>
+    <t>test_majitel\32237.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Roman Jurda, Ing. Juraj Vrábel</t>
+  </si>
+  <si>
+    <t>test_majitel\32330.pdf</t>
+  </si>
+  <si>
+    <t>Peter Gatial, Mgr. Lenka Gatialová</t>
+  </si>
+  <si>
+    <t>test_majitel\17279.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Ivan Lovíšek</t>
+  </si>
+  <si>
+    <t>test_majitel\34013.pdf</t>
+  </si>
+  <si>
+    <t>Ján Samek</t>
+  </si>
+  <si>
+    <t>test_majitel\15269.pdf</t>
+  </si>
+  <si>
+    <t>Roman Danda, Ing. Lubomír Hezina, Ing. Karel Kovář</t>
+  </si>
+  <si>
+    <t>test_majitel\316</t>
+  </si>
+  <si>
+    <t>Ing. Ján Baran</t>
+  </si>
+  <si>
+    <t>test_majitel\102364.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Peter Polakovič</t>
+  </si>
+  <si>
+    <t>test_majitel\17569.pdf</t>
+  </si>
+  <si>
+    <t>Julius Prüger</t>
+  </si>
+  <si>
+    <t>test_majitel\115370</t>
+  </si>
+  <si>
+    <t>Jozef Žido</t>
+  </si>
+  <si>
+    <t>test_majitel\102472.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Marian Mojžiš</t>
+  </si>
+  <si>
+    <t>test_majitel\5396.pdf</t>
+  </si>
+  <si>
+    <t>PhDr. Daniel Dobrovič</t>
+  </si>
+  <si>
+    <t>test_majitel\16656.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Vladimír Bugár, Ing. Jozef Kuruc</t>
+  </si>
+  <si>
+    <t>test_majitel\6157.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Jozef Čapkovič</t>
+  </si>
+  <si>
+    <t>test_majitel\69727.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Radoslav Lackovič</t>
+  </si>
+  <si>
+    <t>test_majitel\72393.pdf</t>
+  </si>
+  <si>
+    <t>Soňa Ružanská</t>
+  </si>
+  <si>
+    <t>test_majitel\39936.pdf</t>
+  </si>
+  <si>
+    <t>Juraj Ostrolucký, Róbert Fertály</t>
+  </si>
+  <si>
+    <t>test_majitel\58782.pdf</t>
+  </si>
+  <si>
+    <t>Pieter Ján Kleibergen</t>
+  </si>
+  <si>
+    <t>test_majitel\64582.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Zuzana Klimeková</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +585,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -493,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -516,13 +643,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -806,8 +936,8 @@
   <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,7 +1242,7 @@
       <c r="B13" s="8">
         <v>38</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>45232270</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -2041,15 +2171,15 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
@@ -2076,7 +2206,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
-        <f>A53+1</f>
+        <f t="shared" ref="A54:A68" si="1">A53+1</f>
         <v>2</v>
       </c>
       <c r="B54" s="8">
@@ -2100,7 +2230,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
-        <f>A54+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B55" s="8">
@@ -2124,7 +2254,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
-        <f>A55+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B56" s="6"/>
@@ -2132,7 +2262,7 @@
       <c r="D56" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="15"/>
+      <c r="E56" s="14"/>
       <c r="F56" s="7" t="s">
         <v>41</v>
       </c>
@@ -2142,7 +2272,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
-        <f>A56+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B57" s="6"/>
@@ -2150,7 +2280,7 @@
       <c r="D57" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="15"/>
+      <c r="E57" s="14"/>
       <c r="F57" s="7" t="s">
         <v>41</v>
       </c>
@@ -2160,7 +2290,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
-        <f>A57+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B58" s="6"/>
@@ -2168,7 +2298,7 @@
       <c r="D58" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="15"/>
+      <c r="E58" s="14"/>
       <c r="F58" s="7" t="s">
         <v>41</v>
       </c>
@@ -2178,7 +2308,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
-        <f>A58+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B59" s="6"/>
@@ -2186,7 +2316,7 @@
       <c r="D59" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="15"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="7" t="s">
         <v>41</v>
       </c>
@@ -2196,7 +2326,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
-        <f>A59+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B60" s="6"/>
@@ -2204,7 +2334,7 @@
       <c r="D60" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="15"/>
+      <c r="E60" s="14"/>
       <c r="F60" s="7" t="s">
         <v>41</v>
       </c>
@@ -2214,7 +2344,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
-        <f>A60+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B61" s="6"/>
@@ -2222,7 +2352,7 @@
       <c r="D61" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="15"/>
+      <c r="E61" s="14"/>
       <c r="F61" s="7" t="s">
         <v>41</v>
       </c>
@@ -2232,7 +2362,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
-        <f>A61+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B62" s="6"/>
@@ -2240,7 +2370,7 @@
       <c r="D62" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E62" s="15"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="7" t="s">
         <v>41</v>
       </c>
@@ -2250,7 +2380,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
-        <f>A62+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B63" s="6"/>
@@ -2258,7 +2388,7 @@
       <c r="D63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E63" s="15"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="7" t="s">
         <v>41</v>
       </c>
@@ -2268,7 +2398,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
-        <f>A63+1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B64" s="6"/>
@@ -2276,7 +2406,7 @@
       <c r="D64" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="15"/>
+      <c r="E64" s="14"/>
       <c r="F64" s="7" t="s">
         <v>41</v>
       </c>
@@ -2286,7 +2416,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
-        <f>A64+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B65" s="6"/>
@@ -2294,7 +2424,7 @@
       <c r="D65" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E65" s="15"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="7" t="s">
         <v>41</v>
       </c>
@@ -2304,7 +2434,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
-        <f>A65+1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B66" s="6"/>
@@ -2312,7 +2442,7 @@
       <c r="D66" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="15"/>
+      <c r="E66" s="14"/>
       <c r="F66" s="7" t="s">
         <v>41</v>
       </c>
@@ -2322,7 +2452,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
-        <f>A66+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B67" s="6"/>
@@ -2330,7 +2460,7 @@
       <c r="D67" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E67" s="15"/>
+      <c r="E67" s="14"/>
       <c r="F67" s="7" t="s">
         <v>41</v>
       </c>
@@ -2340,7 +2470,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
-        <f>A67+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B68" s="6"/>
@@ -2348,7 +2478,7 @@
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="15"/>
+      <c r="E68" s="14"/>
       <c r="F68" s="7" t="s">
         <v>41</v>
       </c>
@@ -2358,7 +2488,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
-        <f t="shared" ref="A69:A101" si="1">A68+1</f>
+        <f t="shared" ref="A69:A101" si="2">A68+1</f>
         <v>17</v>
       </c>
       <c r="B69" s="6"/>
@@ -2366,7 +2496,7 @@
       <c r="D69" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E69" s="15"/>
+      <c r="E69" s="14"/>
       <c r="F69" s="7" t="s">
         <v>41</v>
       </c>
@@ -2376,7 +2506,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B70" s="6"/>
@@ -2384,7 +2514,7 @@
       <c r="D70" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="15"/>
+      <c r="E70" s="14"/>
       <c r="F70" s="7" t="s">
         <v>41</v>
       </c>
@@ -2394,7 +2524,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B71" s="6"/>
@@ -2402,7 +2532,7 @@
       <c r="D71" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E71" s="15"/>
+      <c r="E71" s="14"/>
       <c r="F71" s="7" t="s">
         <v>41</v>
       </c>
@@ -2412,7 +2542,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B72" s="6"/>
@@ -2420,7 +2550,7 @@
       <c r="D72" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E72" s="15"/>
+      <c r="E72" s="14"/>
       <c r="F72" s="7" t="s">
         <v>41</v>
       </c>
@@ -2430,7 +2560,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B73" s="6"/>
@@ -2438,7 +2568,7 @@
       <c r="D73" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E73" s="15"/>
+      <c r="E73" s="14"/>
       <c r="F73" s="7" t="s">
         <v>41</v>
       </c>
@@ -2448,7 +2578,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="B74" s="6"/>
@@ -2456,7 +2586,7 @@
       <c r="D74" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E74" s="15"/>
+      <c r="E74" s="14"/>
       <c r="F74" s="7" t="s">
         <v>41</v>
       </c>
@@ -2466,7 +2596,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B75" s="6"/>
@@ -2474,7 +2604,7 @@
       <c r="D75" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="15"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="7" t="s">
         <v>41</v>
       </c>
@@ -2484,7 +2614,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B76" s="6"/>
@@ -2492,7 +2622,7 @@
       <c r="D76" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="15"/>
+      <c r="E76" s="14"/>
       <c r="F76" s="7" t="s">
         <v>41</v>
       </c>
@@ -2502,7 +2632,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B77" s="6"/>
@@ -2510,7 +2640,7 @@
       <c r="D77" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="15"/>
+      <c r="E77" s="14"/>
       <c r="F77" s="7" t="s">
         <v>41</v>
       </c>
@@ -2520,7 +2650,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B78" s="6"/>
@@ -2528,7 +2658,7 @@
       <c r="D78" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="15"/>
+      <c r="E78" s="14"/>
       <c r="F78" s="7" t="s">
         <v>41</v>
       </c>
@@ -2538,7 +2668,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B79" s="6"/>
@@ -2546,7 +2676,7 @@
       <c r="D79" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="15"/>
+      <c r="E79" s="14"/>
       <c r="F79" s="7" t="s">
         <v>41</v>
       </c>
@@ -2556,7 +2686,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B80" s="6"/>
@@ -2564,7 +2694,7 @@
       <c r="D80" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="15"/>
+      <c r="E80" s="14"/>
       <c r="F80" s="7" t="s">
         <v>41</v>
       </c>
@@ -2574,7 +2704,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B81" s="6"/>
@@ -2582,7 +2712,7 @@
       <c r="D81" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E81" s="15"/>
+      <c r="E81" s="14"/>
       <c r="F81" s="7" t="s">
         <v>41</v>
       </c>
@@ -2592,7 +2722,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B82" s="6"/>
@@ -2600,7 +2730,7 @@
       <c r="D82" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="15"/>
+      <c r="E82" s="14"/>
       <c r="F82" s="7" t="s">
         <v>41</v>
       </c>
@@ -2610,7 +2740,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B83" s="6"/>
@@ -2618,7 +2748,7 @@
       <c r="D83" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="15"/>
+      <c r="E83" s="14"/>
       <c r="F83" s="7" t="s">
         <v>41</v>
       </c>
@@ -2628,7 +2758,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B84" s="6"/>
@@ -2636,7 +2766,7 @@
       <c r="D84" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E84" s="15"/>
+      <c r="E84" s="14"/>
       <c r="F84" s="7" t="s">
         <v>41</v>
       </c>
@@ -2646,7 +2776,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B85" s="6"/>
@@ -2654,7 +2784,7 @@
       <c r="D85" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E85" s="15"/>
+      <c r="E85" s="14"/>
       <c r="F85" s="7" t="s">
         <v>41</v>
       </c>
@@ -2664,7 +2794,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B86" s="6"/>
@@ -2672,7 +2802,7 @@
       <c r="D86" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E86" s="15"/>
+      <c r="E86" s="14"/>
       <c r="F86" s="7" t="s">
         <v>41</v>
       </c>
@@ -2682,7 +2812,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B87" s="6"/>
@@ -2690,7 +2820,7 @@
       <c r="D87" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E87" s="15"/>
+      <c r="E87" s="14"/>
       <c r="F87" s="7" t="s">
         <v>41</v>
       </c>
@@ -2700,7 +2830,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B88" s="6"/>
@@ -2708,7 +2838,7 @@
       <c r="D88" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E88" s="15"/>
+      <c r="E88" s="14"/>
       <c r="F88" s="7" t="s">
         <v>41</v>
       </c>
@@ -2718,7 +2848,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B89" s="6"/>
@@ -2726,7 +2856,7 @@
       <c r="D89" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E89" s="15"/>
+      <c r="E89" s="14"/>
       <c r="F89" s="7" t="s">
         <v>41</v>
       </c>
@@ -2736,7 +2866,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B90" s="6"/>
@@ -2744,7 +2874,7 @@
       <c r="D90" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E90" s="15"/>
+      <c r="E90" s="14"/>
       <c r="F90" s="7" t="s">
         <v>41</v>
       </c>
@@ -2754,7 +2884,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B91" s="6"/>
@@ -2762,7 +2892,7 @@
       <c r="D91" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E91" s="15"/>
+      <c r="E91" s="14"/>
       <c r="F91" s="7" t="s">
         <v>41</v>
       </c>
@@ -2772,7 +2902,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B92" s="6"/>
@@ -2780,7 +2910,7 @@
       <c r="D92" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="15"/>
+      <c r="E92" s="14"/>
       <c r="F92" s="7" t="s">
         <v>41</v>
       </c>
@@ -2790,7 +2920,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="B93" s="6"/>
@@ -2798,7 +2928,7 @@
       <c r="D93" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E93" s="15"/>
+      <c r="E93" s="14"/>
       <c r="F93" s="7" t="s">
         <v>41</v>
       </c>
@@ -2808,7 +2938,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="B94" s="6"/>
@@ -2816,7 +2946,7 @@
       <c r="D94" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E94" s="15"/>
+      <c r="E94" s="14"/>
       <c r="F94" s="7" t="s">
         <v>41</v>
       </c>
@@ -2826,7 +2956,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="B95" s="6"/>
@@ -2834,7 +2964,7 @@
       <c r="D95" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E95" s="15"/>
+      <c r="E95" s="14"/>
       <c r="F95" s="7" t="s">
         <v>41</v>
       </c>
@@ -2844,7 +2974,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="B96" s="6"/>
@@ -2852,7 +2982,7 @@
       <c r="D96" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E96" s="15"/>
+      <c r="E96" s="14"/>
       <c r="F96" s="7" t="s">
         <v>41</v>
       </c>
@@ -2862,7 +2992,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="B97" s="6"/>
@@ -2870,7 +3000,7 @@
       <c r="D97" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E97" s="15"/>
+      <c r="E97" s="14"/>
       <c r="F97" s="7" t="s">
         <v>41</v>
       </c>
@@ -2880,7 +3010,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="B98" s="6"/>
@@ -2888,7 +3018,7 @@
       <c r="D98" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E98" s="15"/>
+      <c r="E98" s="14"/>
       <c r="F98" s="7" t="s">
         <v>41</v>
       </c>
@@ -2898,7 +3028,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="B99" s="6"/>
@@ -2906,7 +3036,7 @@
       <c r="D99" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E99" s="15"/>
+      <c r="E99" s="14"/>
       <c r="F99" s="7" t="s">
         <v>41</v>
       </c>
@@ -2916,7 +3046,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="B100" s="6"/>
@@ -2924,7 +3054,7 @@
       <c r="D100" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E100" s="15"/>
+      <c r="E100" s="14"/>
       <c r="F100" s="7" t="s">
         <v>41</v>
       </c>
@@ -2934,7 +3064,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="B101" s="6"/>
@@ -2942,7 +3072,7 @@
       <c r="D101" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E101" s="15"/>
+      <c r="E101" s="14"/>
       <c r="F101" s="7" t="s">
         <v>41</v>
       </c>
@@ -2960,7 +3090,7 @@
       <c r="D102" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E102" s="15"/>
+      <c r="E102" s="14"/>
       <c r="F102" s="7" t="s">
         <v>41</v>
       </c>
@@ -2969,15 +3099,15 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="14" t="s">
+      <c r="A103" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="16"/>
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
@@ -3028,7 +3158,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
-        <f t="shared" ref="A106:A153" si="2">A105+1</f>
+        <f t="shared" ref="A106:A153" si="3">A105+1</f>
         <v>3</v>
       </c>
       <c r="B106" s="8">
@@ -3052,7 +3182,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B107" s="8">
@@ -3076,7 +3206,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B108" s="8">
@@ -3100,7 +3230,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B109" s="8">
@@ -3124,7 +3254,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B110" s="8">
@@ -3148,7 +3278,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B111" s="8">
@@ -3172,7 +3302,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B112" s="8">
@@ -3196,7 +3326,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B113" s="8">
@@ -3220,7 +3350,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B114" s="8">
@@ -3242,351 +3372,465 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B115" s="6"/>
-      <c r="C115" s="13"/>
+      <c r="B115" s="17">
+        <v>289</v>
+      </c>
+      <c r="C115" s="17">
+        <v>36499439</v>
+      </c>
       <c r="D115" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E115" s="15"/>
+      <c r="E115" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="F115" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B116" s="6"/>
-      <c r="C116" s="13"/>
+      <c r="B116" s="17">
+        <v>295</v>
+      </c>
+      <c r="C116" s="17">
+        <v>35872926</v>
+      </c>
       <c r="D116" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E116" s="15"/>
+      <c r="E116" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="F116" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B117" s="6"/>
-      <c r="C117" s="13"/>
+      <c r="B117" s="17">
+        <v>302</v>
+      </c>
+      <c r="C117" s="17">
+        <v>35791187</v>
+      </c>
       <c r="D117" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E117" s="15"/>
+      <c r="E117" s="18" t="s">
+        <v>147</v>
+      </c>
       <c r="F117" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B118" s="6"/>
-      <c r="C118" s="13"/>
+      <c r="B118" s="17">
+        <v>307</v>
+      </c>
+      <c r="C118" s="17">
+        <v>31580220</v>
+      </c>
       <c r="D118" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E118" s="15"/>
+      <c r="E118" s="18" t="s">
+        <v>149</v>
+      </c>
       <c r="F118" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B119" s="6"/>
-      <c r="C119" s="13"/>
+      <c r="B119" s="17">
+        <v>312</v>
+      </c>
+      <c r="C119" s="17">
+        <v>47360119</v>
+      </c>
       <c r="D119" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E119" s="15"/>
+      <c r="E119" s="18" t="s">
+        <v>151</v>
+      </c>
       <c r="F119" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B120" s="6"/>
-      <c r="C120" s="13"/>
+      <c r="B120" s="17">
+        <v>316</v>
+      </c>
+      <c r="C120" s="17">
+        <v>36385492</v>
+      </c>
       <c r="D120" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E120" s="15"/>
+      <c r="E120" s="19" t="s">
+        <v>153</v>
+      </c>
       <c r="F120" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B121" s="6"/>
-      <c r="C121" s="13"/>
+      <c r="B121" s="17">
+        <v>317</v>
+      </c>
+      <c r="C121" s="17">
+        <v>44803401</v>
+      </c>
       <c r="D121" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E121" s="15"/>
+      <c r="E121" s="18" t="s">
+        <v>155</v>
+      </c>
       <c r="F121" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B122" s="6"/>
-      <c r="C122" s="13"/>
+      <c r="B122" s="17">
+        <v>332</v>
+      </c>
+      <c r="C122" s="17">
+        <v>48108791</v>
+      </c>
       <c r="D122" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E122" s="15"/>
+      <c r="E122" s="18" t="s">
+        <v>157</v>
+      </c>
       <c r="F122" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B123" s="6"/>
-      <c r="C123" s="13"/>
+      <c r="B123" s="17">
+        <v>350</v>
+      </c>
+      <c r="C123" s="17">
+        <v>612758</v>
+      </c>
       <c r="D123" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E123" s="15"/>
+      <c r="E123" s="18" t="s">
+        <v>159</v>
+      </c>
       <c r="F123" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B124" s="6"/>
-      <c r="C124" s="13"/>
+      <c r="B124" s="17">
+        <v>367</v>
+      </c>
+      <c r="C124" s="17">
+        <v>31444253</v>
+      </c>
       <c r="D124" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E124" s="15"/>
+      <c r="E124" s="18" t="s">
+        <v>161</v>
+      </c>
       <c r="F124" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B125" s="6"/>
-      <c r="C125" s="13"/>
+      <c r="B125" s="17">
+        <v>368</v>
+      </c>
+      <c r="C125" s="17">
+        <v>31415261</v>
+      </c>
       <c r="D125" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E125" s="15"/>
+      <c r="E125" s="18" t="s">
+        <v>163</v>
+      </c>
       <c r="F125" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B126" s="6"/>
-      <c r="C126" s="13"/>
+      <c r="B126" s="17">
+        <v>369</v>
+      </c>
+      <c r="C126" s="17">
+        <v>43818030</v>
+      </c>
       <c r="D126" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E126" s="15"/>
+      <c r="E126" s="18" t="s">
+        <v>165</v>
+      </c>
       <c r="F126" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B127" s="6"/>
-      <c r="C127" s="13"/>
+      <c r="B127" s="17">
+        <v>373</v>
+      </c>
+      <c r="C127" s="17">
+        <v>36526606</v>
+      </c>
       <c r="D127" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E127" s="15"/>
+      <c r="E127" s="18" t="s">
+        <v>167</v>
+      </c>
       <c r="F127" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B128" s="6"/>
-      <c r="C128" s="13"/>
+      <c r="B128" s="17">
+        <v>380</v>
+      </c>
+      <c r="C128" s="17">
+        <v>44295588</v>
+      </c>
       <c r="D128" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E128" s="15"/>
+      <c r="E128" s="18" t="s">
+        <v>169</v>
+      </c>
       <c r="F128" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B129" s="6"/>
-      <c r="C129" s="13"/>
+      <c r="B129" s="17">
+        <v>382</v>
+      </c>
+      <c r="C129" s="17">
+        <v>36462110</v>
+      </c>
       <c r="D129" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E129" s="15"/>
+      <c r="E129" s="18" t="s">
+        <v>171</v>
+      </c>
       <c r="F129" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B130" s="6"/>
-      <c r="C130" s="13"/>
+      <c r="B130" s="17">
+        <v>389</v>
+      </c>
+      <c r="C130" s="17">
+        <v>44966873</v>
+      </c>
       <c r="D130" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E130" s="15"/>
+      <c r="E130" s="18" t="s">
+        <v>173</v>
+      </c>
       <c r="F130" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B131" s="6"/>
-      <c r="C131" s="13"/>
+      <c r="B131" s="17">
+        <v>390</v>
+      </c>
+      <c r="C131" s="17">
+        <v>691542</v>
+      </c>
       <c r="D131" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E131" s="15"/>
+      <c r="E131" s="19" t="s">
+        <v>175</v>
+      </c>
       <c r="F131" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B132" s="6"/>
-      <c r="C132" s="13"/>
+      <c r="B132" s="17">
+        <v>452</v>
+      </c>
+      <c r="C132" s="17">
+        <v>31351611</v>
+      </c>
       <c r="D132" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E132" s="15"/>
+      <c r="E132" s="18" t="s">
+        <v>177</v>
+      </c>
       <c r="F132" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B133" s="6"/>
-      <c r="C133" s="13"/>
+      <c r="B133" s="17">
+        <v>481</v>
+      </c>
+      <c r="C133" s="17">
+        <v>697591</v>
+      </c>
       <c r="D133" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E133" s="15"/>
+      <c r="E133" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="F133" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B134" s="6"/>
@@ -3594,7 +3838,7 @@
       <c r="D134" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E134" s="15"/>
+      <c r="E134" s="14"/>
       <c r="F134" s="7" t="s">
         <v>7</v>
       </c>
@@ -3604,7 +3848,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B135" s="6"/>
@@ -3612,7 +3856,7 @@
       <c r="D135" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E135" s="15"/>
+      <c r="E135" s="14"/>
       <c r="F135" s="7" t="s">
         <v>7</v>
       </c>
@@ -3622,7 +3866,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B136" s="6"/>
@@ -3630,7 +3874,7 @@
       <c r="D136" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E136" s="15"/>
+      <c r="E136" s="14"/>
       <c r="F136" s="7" t="s">
         <v>7</v>
       </c>
@@ -3640,7 +3884,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B137" s="6"/>
@@ -3648,7 +3892,7 @@
       <c r="D137" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E137" s="15"/>
+      <c r="E137" s="14"/>
       <c r="F137" s="7" t="s">
         <v>7</v>
       </c>
@@ -3658,7 +3902,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B138" s="6"/>
@@ -3666,7 +3910,7 @@
       <c r="D138" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E138" s="15"/>
+      <c r="E138" s="14"/>
       <c r="F138" s="7" t="s">
         <v>7</v>
       </c>
@@ -3676,7 +3920,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B139" s="6"/>
@@ -3684,7 +3928,7 @@
       <c r="D139" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E139" s="15"/>
+      <c r="E139" s="14"/>
       <c r="F139" s="7" t="s">
         <v>7</v>
       </c>
@@ -3694,7 +3938,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="B140" s="6"/>
@@ -3702,7 +3946,7 @@
       <c r="D140" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E140" s="15"/>
+      <c r="E140" s="14"/>
       <c r="F140" s="7" t="s">
         <v>7</v>
       </c>
@@ -3712,7 +3956,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="B141" s="6"/>
@@ -3720,7 +3964,7 @@
       <c r="D141" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E141" s="15"/>
+      <c r="E141" s="14"/>
       <c r="F141" s="7" t="s">
         <v>7</v>
       </c>
@@ -3730,7 +3974,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="B142" s="6"/>
@@ -3738,7 +3982,7 @@
       <c r="D142" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E142" s="15"/>
+      <c r="E142" s="14"/>
       <c r="F142" s="7" t="s">
         <v>7</v>
       </c>
@@ -3748,7 +3992,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="B143" s="6"/>
@@ -3756,7 +4000,7 @@
       <c r="D143" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E143" s="15"/>
+      <c r="E143" s="14"/>
       <c r="F143" s="7" t="s">
         <v>7</v>
       </c>
@@ -3766,7 +4010,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="B144" s="6"/>
@@ -3774,7 +4018,7 @@
       <c r="D144" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E144" s="15"/>
+      <c r="E144" s="14"/>
       <c r="F144" s="7" t="s">
         <v>7</v>
       </c>
@@ -3784,7 +4028,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="B145" s="6"/>
@@ -3792,7 +4036,7 @@
       <c r="D145" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E145" s="15"/>
+      <c r="E145" s="14"/>
       <c r="F145" s="7" t="s">
         <v>7</v>
       </c>
@@ -3802,7 +4046,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B146" s="6"/>
@@ -3810,7 +4054,7 @@
       <c r="D146" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E146" s="15"/>
+      <c r="E146" s="14"/>
       <c r="F146" s="7" t="s">
         <v>7</v>
       </c>
@@ -3820,7 +4064,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="B147" s="6"/>
@@ -3828,7 +4072,7 @@
       <c r="D147" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E147" s="15"/>
+      <c r="E147" s="14"/>
       <c r="F147" s="7" t="s">
         <v>7</v>
       </c>
@@ -3838,7 +4082,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="B148" s="6"/>
@@ -3846,7 +4090,7 @@
       <c r="D148" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E148" s="15"/>
+      <c r="E148" s="14"/>
       <c r="F148" s="7" t="s">
         <v>7</v>
       </c>
@@ -3856,7 +4100,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="B149" s="6"/>
@@ -3864,7 +4108,7 @@
       <c r="D149" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E149" s="15"/>
+      <c r="E149" s="14"/>
       <c r="F149" s="7" t="s">
         <v>7</v>
       </c>
@@ -3874,7 +4118,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="B150" s="6"/>
@@ -3882,7 +4126,7 @@
       <c r="D150" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E150" s="15"/>
+      <c r="E150" s="14"/>
       <c r="F150" s="7" t="s">
         <v>7</v>
       </c>
@@ -3892,7 +4136,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="B151" s="6"/>
@@ -3900,7 +4144,7 @@
       <c r="D151" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E151" s="15"/>
+      <c r="E151" s="14"/>
       <c r="F151" s="7" t="s">
         <v>7</v>
       </c>
@@ -3910,7 +4154,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="B152" s="6"/>
@@ -3918,7 +4162,7 @@
       <c r="D152" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E152" s="15"/>
+      <c r="E152" s="14"/>
       <c r="F152" s="7" t="s">
         <v>7</v>
       </c>
@@ -3928,7 +4172,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="B153" s="6"/>
@@ -3936,7 +4180,7 @@
       <c r="D153" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E153" s="15"/>
+      <c r="E153" s="14"/>
       <c r="F153" s="7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
items to dataset added
</commit_message>
<xml_diff>
--- a/Dataset/list.xlsx
+++ b/Dataset/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMFI\1. semester\Bakalárka\na_git\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6688ACCC-992E-411D-B69F-ABD963F1D41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99D1FED-5618-4387-B06B-0CB47114F083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="238">
   <si>
     <t>Číslo vložky</t>
   </si>
@@ -699,7 +699,46 @@
     <t>Ing. Ľubomír Gúčik</t>
   </si>
   <si>
-    <t>po 619</t>
+    <t>Platní, no bez overani:</t>
+  </si>
+  <si>
+    <t>https://rpvs.gov.sk/rpvs/Partner/Partner/Detail/646</t>
+  </si>
+  <si>
+    <t>statutar\26989.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Pavel Bízek, Ing. Milan Konôpka</t>
+  </si>
+  <si>
+    <t>statutar\93052.pdf</t>
+  </si>
+  <si>
+    <t>Mgr. Anton Behan, Ing. Adrián Csuba</t>
+  </si>
+  <si>
+    <t>46529233</t>
+  </si>
+  <si>
+    <t>statutar\115604.pdf</t>
+  </si>
+  <si>
+    <t>Ing. Janka Olejová</t>
+  </si>
+  <si>
+    <t>statutar\103005.pdf</t>
+  </si>
+  <si>
+    <t>prof. Ing Miroslav Fikar DrSc.</t>
+  </si>
+  <si>
+    <t>statutar\118476.pdf</t>
+  </si>
+  <si>
+    <t>Sun Yong Hwang</t>
+  </si>
+  <si>
+    <t>po 959</t>
   </si>
 </sst>
 </file>
@@ -806,13 +845,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -1093,11 +1132,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:P153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,7 +1147,7 @@
     <col min="6" max="6" width="11" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1154,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1178,7 +1217,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A50" si="0">A3+1</f>
         <v>3</v>
@@ -1202,7 +1241,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1225,11 +1264,8 @@
       <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1253,7 +1289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1277,7 +1313,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1300,8 +1336,11 @@
       <c r="G8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="P8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1324,8 +1363,11 @@
       <c r="G9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1349,7 +1391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1373,7 +1415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1397,7 +1439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1421,7 +1463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1445,7 +1487,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1469,7 +1511,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2261,7 +2303,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2285,7 +2327,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2309,7 +2351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <f>A50+1</f>
         <v>50</v>
@@ -2333,18 +2375,18 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>1</v>
       </c>
@@ -2367,7 +2409,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <f t="shared" ref="A54:A68" si="1">A53+1</f>
         <v>2</v>
@@ -2391,7 +2433,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -2415,7 +2457,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2439,7 +2481,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2463,97 +2505,130 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="13"/>
+      <c r="B58" s="16">
+        <v>710</v>
+      </c>
+      <c r="C58" s="16">
+        <v>31399614</v>
+      </c>
       <c r="D58" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="14"/>
+      <c r="E58" s="12" t="s">
+        <v>227</v>
+      </c>
       <c r="F58" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="13"/>
+      <c r="B59" s="16">
+        <v>683</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>230</v>
+      </c>
       <c r="D59" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="14"/>
+      <c r="E59" s="12" t="s">
+        <v>229</v>
+      </c>
       <c r="F59" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+      <c r="K59" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="13"/>
+      <c r="B60" s="16">
+        <v>814</v>
+      </c>
+      <c r="C60" s="16">
+        <v>165506</v>
+      </c>
       <c r="D60" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="14"/>
+      <c r="E60" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="F60" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="13"/>
+      <c r="B61" s="16">
+        <v>830</v>
+      </c>
+      <c r="C61" s="16">
+        <v>397687</v>
+      </c>
       <c r="D61" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="14"/>
+      <c r="E61" s="17" t="s">
+        <v>234</v>
+      </c>
       <c r="F61" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="13"/>
+      <c r="B62" s="16">
+        <v>949</v>
+      </c>
+      <c r="C62" s="16">
+        <v>28399757</v>
+      </c>
       <c r="D62" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E62" s="14"/>
+      <c r="E62" s="17" t="s">
+        <v>236</v>
+      </c>
       <c r="F62" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2571,7 +2646,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3274,15 +3349,15 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="19" t="s">
+      <c r="A103" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B103" s="19"/>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19"/>
-      <c r="G103" s="19"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
@@ -4041,7 +4116,7 @@
       <c r="D135" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E135" s="20" t="s">
+      <c r="E135" s="19" t="s">
         <v>182</v>
       </c>
       <c r="F135" s="7" t="s">
@@ -4113,7 +4188,7 @@
       <c r="D138" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E138" s="21" t="s">
+      <c r="E138" s="20" t="s">
         <v>188</v>
       </c>
       <c r="F138" s="7" t="s">

</xml_diff>

<commit_message>
rotated img detection implemented
</commit_message>
<xml_diff>
--- a/Dataset/list.xlsx
+++ b/Dataset/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMFI\Bakalárka\na_git\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20849694-8004-4339-A07A-AD49F2235C55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE52C12-1570-4BF9-859D-620147FFF1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="361">
   <si>
     <t>Číslo vložky</t>
   </si>
@@ -1102,6 +1102,12 @@
   </si>
   <si>
     <t>po 4317</t>
+  </si>
+  <si>
+    <t>vymazať - nie je štatutár</t>
+  </si>
+  <si>
+    <t>vymazať - nie je štatutár, keďže Sečka skutočne ovláda a kontroluje ...</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1514,8 @@
   <dimension ref="A1:P207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q169" sqref="Q169"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3480,6 +3486,9 @@
       <c r="G82" s="6" t="s">
         <v>278</v>
       </c>
+      <c r="I82" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="83" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
@@ -3552,6 +3561,9 @@
       <c r="G85" s="6" t="s">
         <v>284</v>
       </c>
+      <c r="I85" t="s">
+        <v>360</v>
+      </c>
       <c r="L85" t="s">
         <v>294</v>
       </c>
@@ -3626,6 +3638,9 @@
       </c>
       <c r="G88" s="6" t="s">
         <v>291</v>
+      </c>
+      <c r="I88" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
more KUVs preprocessing fixed
</commit_message>
<xml_diff>
--- a/Dataset/list.xlsx
+++ b/Dataset/list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMFI\Bakalárka\na_git\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE52C12-1570-4BF9-859D-620147FFF1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F4600E-A650-48EE-AAA9-21E70DA156C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -1514,8 +1514,8 @@
   <dimension ref="A1:P207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I86" sqref="I86"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
redudant code deleted, misclassified pdf from pdf replaced
</commit_message>
<xml_diff>
--- a/Dataset/list.xlsx
+++ b/Dataset/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FMFI\Bakalárka\na_git\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F4600E-A650-48EE-AAA9-21E70DA156C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D40F92-1423-49B5-9BDC-CFE45C9D60D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="353">
   <si>
     <t>Číslo vložky</t>
   </si>
@@ -861,12 +861,6 @@
     <t>Andreas Jozef Brun, Teemu Tapani Airaksinen</t>
   </si>
   <si>
-    <t>statutar\107830.pdf</t>
-  </si>
-  <si>
-    <t>Helena Maria Stjernholm, Erik A Elzvik, Jon Fredrick Baksaas, Jan Ove Mikael Carlson, Bo Kjell-Ȁke Soting, Inge Roger Svensson, Jacob Wallenberg, Erik Börje Ekholm, Nora Denzel, Kristin Sue Rinne, Carl Fredrik Harry Jejdling, Kurt Åke Jofs, Lars Erik Torbjörn Nyman, Ronnie Frans Ghislain Leten</t>
-  </si>
-  <si>
     <t>statutar\22455.pdf</t>
   </si>
   <si>
@@ -879,12 +873,6 @@
     <t>RNDr. Martin Ružinský PhD., Ing. Ján Horkovič, Ing. Milan Rác MBA, Ing. Marián Lokša, Ing. Peter Zelinka, Ing. Peter Ufnár, Ing. Katarína Vršanská, Ing. Ivan Bilohuščin</t>
   </si>
   <si>
-    <t>statutar\30031.pdf</t>
-  </si>
-  <si>
-    <t>ThDr. Štefan Sečka PhD.</t>
-  </si>
-  <si>
     <t>statutar\98669.pdf</t>
   </si>
   <si>
@@ -900,18 +888,12 @@
     <t>Jan Knyttl, Ing. Tomáš Belavý</t>
   </si>
   <si>
-    <t>statutar\18934.pdf</t>
-  </si>
-  <si>
     <t>statutar\38551.pdf</t>
   </si>
   <si>
     <t>Ing. Jindřich Frič Ph.D.</t>
   </si>
   <si>
-    <t>možno bude treba odstraniť tých, ktorý sú KUV podľa 6a ods. 1</t>
-  </si>
-  <si>
     <t>statutar\23053.pdf</t>
   </si>
   <si>
@@ -1102,12 +1084,6 @@
   </si>
   <si>
     <t>po 4317</t>
-  </si>
-  <si>
-    <t>vymazať - nie je štatutár</t>
-  </si>
-  <si>
-    <t>vymazať - nie je štatutár, keďže Sečka skutočne ovláda a kontroluje ...</t>
   </si>
 </sst>
 </file>
@@ -1513,9 +1489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K174" sqref="K174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3439,7 +3415,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3463,34 +3439,28 @@
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B82" s="15">
-        <v>1945</v>
+        <v>4298</v>
       </c>
       <c r="C82" s="15">
-        <v>31344046</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="I82" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>44750498</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G82" s="21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -3505,16 +3475,16 @@
         <v>5</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -3529,46 +3499,40 @@
         <v>5</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F84" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B85" s="15">
-        <v>2136</v>
+        <v>4222</v>
       </c>
       <c r="C85" s="15">
-        <v>35514221</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E85" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="I85" t="s">
-        <v>360</v>
-      </c>
-      <c r="L85" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>35774738</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G85" s="21" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -3577,22 +3541,22 @@
         <v>2210</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -3607,43 +3571,40 @@
         <v>5</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B88" s="15">
-        <v>2308</v>
+        <v>4202</v>
       </c>
       <c r="C88" s="15">
-        <v>17083851</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E88" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="I88" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>36277215</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G88" s="21" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -3658,16 +3619,16 @@
         <v>5</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -3682,16 +3643,16 @@
         <v>5</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -3706,16 +3667,16 @@
         <v>5</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -3730,16 +3691,16 @@
         <v>5</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -3748,22 +3709,22 @@
         <v>2533</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -3778,16 +3739,16 @@
         <v>5</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -3802,16 +3763,16 @@
         <v>5</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -3826,13 +3787,13 @@
         <v>5</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3850,13 +3811,13 @@
         <v>5</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3874,13 +3835,13 @@
         <v>5</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3898,13 +3859,13 @@
         <v>5</v>
       </c>
       <c r="E99" s="17" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3922,13 +3883,13 @@
         <v>5</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3946,13 +3907,13 @@
         <v>5</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="F101" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3970,13 +3931,13 @@
         <v>5</v>
       </c>
       <c r="E102" s="17" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -5238,13 +5199,13 @@
         <v>5</v>
       </c>
       <c r="E156" s="17" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G156" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5262,13 +5223,13 @@
         <v>5</v>
       </c>
       <c r="E157" s="16" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G157" s="21" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5286,13 +5247,13 @@
         <v>5</v>
       </c>
       <c r="E158" s="16" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G158" s="21" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5310,16 +5271,16 @@
         <v>5</v>
       </c>
       <c r="E159" s="17" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G159" s="21" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="L159" s="15" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5337,13 +5298,13 @@
         <v>5</v>
       </c>
       <c r="E160" s="17" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G160" s="21" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="161" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5361,13 +5322,13 @@
         <v>5</v>
       </c>
       <c r="E161" s="17" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G161" s="21" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="162" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5385,13 +5346,13 @@
         <v>5</v>
       </c>
       <c r="E162" s="16" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G162" s="21" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="163" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5409,13 +5370,13 @@
         <v>5</v>
       </c>
       <c r="E163" s="16" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G163" s="21" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="164" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5433,13 +5394,13 @@
         <v>5</v>
       </c>
       <c r="E164" s="17" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G164" s="21" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="165" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5457,13 +5418,13 @@
         <v>5</v>
       </c>
       <c r="E165" s="17" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G165" s="21" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="166" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5481,16 +5442,16 @@
         <v>5</v>
       </c>
       <c r="E166" s="17" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G166" s="21" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="K166" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="167" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5508,13 +5469,13 @@
         <v>5</v>
       </c>
       <c r="E167" s="16" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G167" s="21" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="168" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5532,74 +5493,50 @@
         <v>5</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G168" s="21" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="B169" s="15">
-        <v>4202</v>
-      </c>
-      <c r="C169" s="15">
-        <v>36277215</v>
-      </c>
       <c r="D169" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E169" s="17" t="s">
-        <v>354</v>
-      </c>
       <c r="F169" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G169" s="21" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="B170" s="15">
-        <v>4222</v>
-      </c>
-      <c r="C170" s="15">
-        <v>35774738</v>
-      </c>
       <c r="D170" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E170" s="17" t="s">
-        <v>356</v>
-      </c>
       <c r="F170" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G170" s="21" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="B171" s="15">
-        <v>4298</v>
-      </c>
-      <c r="C171" s="15">
-        <v>44750498</v>
-      </c>
       <c r="D171" s="21" t="s">
         <v>5</v>
       </c>
@@ -5607,7 +5544,7 @@
         <v>41</v>
       </c>
       <c r="G171" s="21" t="s">
-        <v>357</v>
+        <v>269</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
@@ -6107,18 +6044,18 @@
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="L206" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="L207" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>